<commit_message>
optimized support for composite primary key
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SalesOrders_2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="SampleNumbers" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="MyLinks" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Complex UTF-8 key value àèò§" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="51">
   <si>
     <t xml:space="preserve">Order_id</t>
   </si>
@@ -405,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>307080</xdr:colOff>
+      <xdr:colOff>305640</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>82080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -417,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="921960" cy="769320"/>
+          <a:ext cx="920520" cy="767880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -461,7 +462,7 @@
             </a:rPr>
             <a:t>3/4</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -484,7 +485,7 @@
             </a:rPr>
             <a:t>02345</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -507,7 +508,7 @@
             </a:rPr>
             <a:t>1-3</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -525,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -604,10 +605,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>19.99</v>
+        <v>18.99</v>
       </c>
       <c r="H3" s="8" t="n">
         <v>999.5</v>
@@ -1682,10 +1683,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1697,11 +1698,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -2854,10 +2855,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Pagina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2873,7 +2874,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5949,7 +5950,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5969,7 +5970,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -34018,10 +34019,1182 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;Lwww.contextures.com&amp;R&amp;D</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>43471</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>189.05</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>43488</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>18.99</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>999.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>43505</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>179.64</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>43522</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>539.73</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>43539</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>167.44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>43556</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>299.4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>43573</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>149.25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>43590</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>43607</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>63.68</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>43624</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>539.4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>43641</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>43658</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>57.71</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>43675</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>81</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <v>1619.19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>43692</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H15" s="8" t="n">
+        <v>174.65</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>43709</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="H16" s="8" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>43726</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>255.84</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>43743</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H18" s="8" t="n">
+        <v>251.72</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>43760</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>575.36</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>43777</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H20" s="8" t="n">
+        <v>299.85</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>43794</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <v>96</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H21" s="8" t="n">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>43811</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>67</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H22" s="8" t="n">
+        <v>86.43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>43828</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>74</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="H23" s="8" t="n">
+        <v>1183.26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="n">
+        <v>43845</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H24" s="8" t="n">
+        <v>413.54</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>43862</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>87</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="H25" s="8" t="n">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="n">
+        <v>43879</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G26" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H26" s="8" t="n">
+        <v>19.96</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>43897</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H27" s="8" t="n">
+        <v>139.93</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="n">
+        <v>43914</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H28" s="8" t="n">
+        <v>249.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>43931</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H29" s="8" t="n">
+        <v>131.34</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="n">
+        <v>43948</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>96</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H30" s="8" t="n">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>43965</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="G31" s="7" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H31" s="8" t="n">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="n">
+        <v>43982</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="H32" s="8" t="n">
+        <v>719.2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>43999</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="H33" s="8" t="n">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="n">
+        <v>44016</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>62</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H34" s="8" t="n">
+        <v>309.38</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <v>12.49</v>
+      </c>
+      <c r="H35" s="8" t="n">
+        <v>686.95</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="n">
+        <v>44050</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <v>23.95</v>
+      </c>
+      <c r="H36" s="8" t="n">
+        <v>1005.9</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>44067</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <v>275</v>
+      </c>
+      <c r="H37" s="8" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="n">
+        <v>44084</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H38" s="8" t="n">
+        <v>9.03</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>44101</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>76</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="H39" s="8" t="n">
+        <v>151.24</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="n">
+        <v>44118</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="G40" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H40" s="8" t="n">
+        <v>1139.43</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>44135</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G41" s="7" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="H41" s="8" t="n">
+        <v>18.06</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="n">
+        <v>44152</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G42" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H42" s="8" t="n">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>44169</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>94</v>
+      </c>
+      <c r="G43" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H43" s="8" t="n">
+        <v>1879.06</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="n">
+        <v>44186</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="G44" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H44" s="8" t="n">
+        <v>139.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
controller object is more in control ;-)
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -406,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>305640</xdr:colOff>
+      <xdr:colOff>305280</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -418,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="920520" cy="767880"/>
+          <a:ext cx="920160" cy="767520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -462,7 +462,7 @@
             </a:rPr>
             <a:t>3/4</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -485,7 +485,7 @@
             </a:rPr>
             <a:t>02345</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -508,7 +508,7 @@
             </a:rPr>
             <a:t>1-3</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -527,10 +527,10 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -579,7 +579,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>1.99</v>
@@ -1702,7 +1702,7 @@
       <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -2874,7 +2874,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5970,7 +5970,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -34038,7 +34038,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>

</xml_diff>

<commit_message>
refactor methods involved in importing from xlsx
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="51">
   <si>
     <t xml:space="preserve">Order_id</t>
   </si>
@@ -406,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>305280</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -418,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="920160" cy="767520"/>
+          <a:ext cx="918720" cy="766080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -1696,13 +1696,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -1864,994 +1864,154 @@
         <v>167.44</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>43556</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>299.4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>43573</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>149.25</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>43590</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>449.1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>43607</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>63.68</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>43624</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="G11" s="7" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>539.4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>43641</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="G12" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>449.1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>43658</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="G13" s="7" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>57.71</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>43675</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="G14" s="7" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>1619.19</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>43692</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="G15" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H15" s="8" t="n">
-        <v>174.65</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>43709</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>125</v>
-      </c>
-      <c r="H16" s="8" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>43726</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="G17" s="7" t="n">
-        <v>15.99</v>
-      </c>
-      <c r="H17" s="8" t="n">
-        <v>255.84</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>43743</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="G18" s="7" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H18" s="8" t="n">
-        <v>251.72</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="n">
-        <v>43760</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="G19" s="7" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H19" s="8" t="n">
-        <v>575.36</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="n">
-        <v>43777</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="G20" s="7" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="H20" s="8" t="n">
-        <v>299.85</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="n">
-        <v>43794</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="G21" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H21" s="8" t="n">
-        <v>479.04</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="n">
-        <v>43811</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="5" t="n">
-        <v>67</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="H22" s="8" t="n">
-        <v>86.43</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="n">
-        <v>43828</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>74</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>15.99</v>
-      </c>
-      <c r="H23" s="8" t="n">
-        <v>1183.26</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="n">
-        <v>43845</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>46</v>
-      </c>
-      <c r="G24" s="7" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H24" s="8" t="n">
-        <v>413.54</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="n">
-        <v>43862</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>87</v>
-      </c>
-      <c r="G25" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="H25" s="8" t="n">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>43879</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H26" s="8" t="n">
-        <v>19.96</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="n">
-        <v>43897</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G27" s="7" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="H27" s="8" t="n">
-        <v>139.93</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="n">
-        <v>43914</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="G28" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H28" s="8" t="n">
-        <v>249.5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="n">
-        <v>43931</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>66</v>
-      </c>
-      <c r="G29" s="7" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="H29" s="8" t="n">
-        <v>131.34</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="n">
-        <v>43948</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H30" s="8" t="n">
-        <v>479.04</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="n">
-        <v>43965</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="G31" s="7" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="H31" s="8" t="n">
-        <v>68.37</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4" t="n">
-        <v>43982</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>8.99</v>
-      </c>
-      <c r="H32" s="8" t="n">
-        <v>719.2</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="4" t="n">
-        <v>43999</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G33" s="7" t="n">
-        <v>125</v>
-      </c>
-      <c r="H33" s="8" t="n">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="4" t="n">
-        <v>44016</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>62</v>
-      </c>
-      <c r="G34" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H34" s="8" t="n">
-        <v>309.38</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="4" t="n">
-        <v>44033</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="G35" s="7" t="n">
-        <v>12.49</v>
-      </c>
-      <c r="H35" s="8" t="n">
-        <v>686.95</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" s="4" t="n">
-        <v>44050</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="5" t="n">
-        <v>42</v>
-      </c>
-      <c r="G36" s="7" t="n">
-        <v>23.95</v>
-      </c>
-      <c r="H36" s="8" t="n">
-        <v>1005.9</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="n">
-        <v>44067</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G37" s="7" t="n">
-        <v>275</v>
-      </c>
-      <c r="H37" s="8" t="n">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>44084</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G38" s="7" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="H38" s="8" t="n">
-        <v>9.03</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4" t="n">
-        <v>44101</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="G39" s="7" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="H39" s="8" t="n">
-        <v>151.24</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4" t="n">
-        <v>44118</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="G40" s="7" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="H40" s="8" t="n">
-        <v>1139.43</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" s="4" t="n">
-        <v>44135</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="G41" s="7" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="H41" s="8" t="n">
-        <v>18.06</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="n">
-        <v>44152</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="G42" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H42" s="8" t="n">
-        <v>54.89</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" s="4" t="n">
-        <v>44169</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="5" t="n">
-        <v>94</v>
-      </c>
-      <c r="G43" s="7" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="H43" s="8" t="n">
-        <v>1879.06</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="4" t="n">
-        <v>44186</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="5" t="n">
-        <v>28</v>
-      </c>
-      <c r="G44" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H44" s="8" t="n">
-        <v>139.72</v>
-      </c>
-    </row>
+    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2874,7 +2034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5970,7 +5130,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -34034,11 +33194,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -34087,10 +33247,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>1.99</v>
+        <v>4.99</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>189.05</v>

</xml_diff>

<commit_message>
no primary key test
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" state="visible" r:id="rId2"/>
@@ -406,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>303840</xdr:colOff>
+      <xdr:colOff>303480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -418,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="918720" cy="766080"/>
+          <a:ext cx="918360" cy="765720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -440,7 +440,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -526,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -631,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>36</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="7" t="n">
         <v>4.99</v>
@@ -1702,7 +1702,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -2034,7 +2034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5109,7 +5109,7 @@
     <hyperlink ref="C13" r:id="rId1" location="numberdate" display="Data Entry Tips"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5130,7 +5130,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -33178,7 +33178,7 @@
     <hyperlink ref="B12" r:id="rId6" display="Contextures Recommends"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -33194,11 +33194,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>

</xml_diff>

<commit_message>
modified how to declare the header row, see docs
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" state="visible" r:id="rId2"/>
@@ -406,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>303480</xdr:colOff>
+      <xdr:colOff>303120</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -418,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="918360" cy="765720"/>
+          <a:ext cx="918000" cy="765360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -1702,7 +1702,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -2034,7 +2034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5130,7 +5130,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -33192,440 +33192,388 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A3:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>43471</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>189.05</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>43488</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>18.99</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>999.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>43505</v>
+        <v>43471</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>36</v>
+        <v>1000</v>
       </c>
       <c r="G4" s="7" t="n">
         <v>4.99</v>
       </c>
       <c r="H4" s="8" t="n">
-        <v>179.64</v>
+        <v>189.05</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>43522</v>
+        <v>43488</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>19.99</v>
+        <v>18.99</v>
       </c>
       <c r="H5" s="8" t="n">
-        <v>539.73</v>
+        <v>999.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>43539</v>
+        <v>43505</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>2.99</v>
+        <v>4.99</v>
       </c>
       <c r="H6" s="8" t="n">
-        <v>167.44</v>
+        <v>179.64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>43556</v>
+        <v>43522</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="n">
-        <v>4.99</v>
+        <v>19.99</v>
       </c>
       <c r="H7" s="8" t="n">
-        <v>299.4</v>
+        <v>539.73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>43573</v>
+        <v>43539</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>1.99</v>
+        <v>2.99</v>
       </c>
       <c r="H8" s="8" t="n">
-        <v>149.25</v>
+        <v>167.44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>43556</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>43590</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G9" s="7" t="n">
         <v>4.99</v>
       </c>
       <c r="H9" s="8" t="n">
-        <v>449.1</v>
+        <v>299.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4" t="n">
-        <v>43607</v>
+        <v>43573</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="G10" s="7" t="n">
         <v>1.99</v>
       </c>
       <c r="H10" s="8" t="n">
-        <v>63.68</v>
+        <v>149.25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="n">
-        <v>43624</v>
+        <v>43590</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>8.99</v>
+        <v>4.99</v>
       </c>
       <c r="H11" s="8" t="n">
-        <v>539.4</v>
+        <v>449.1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="n">
-        <v>43641</v>
+        <v>43607</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>4.99</v>
+        <v>1.99</v>
       </c>
       <c r="H12" s="8" t="n">
-        <v>449.1</v>
+        <v>63.68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4" t="n">
-        <v>43658</v>
+        <v>43624</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>1.99</v>
+        <v>8.99</v>
       </c>
       <c r="H13" s="8" t="n">
-        <v>57.71</v>
+        <v>539.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>43641</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="n">
-        <v>43675</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="F14" s="5" t="n">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>19.99</v>
+        <v>4.99</v>
       </c>
       <c r="H14" s="8" t="n">
-        <v>1619.19</v>
+        <v>449.1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4" t="n">
-        <v>43692</v>
+        <v>43658</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>4.99</v>
+        <v>1.99</v>
       </c>
       <c r="H15" s="8" t="n">
-        <v>174.65</v>
+        <v>57.71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="n">
-        <v>43709</v>
+        <v>43675</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>125</v>
+        <v>19.99</v>
       </c>
       <c r="H16" s="8" t="n">
-        <v>250</v>
+        <v>1619.19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="n">
-        <v>43726</v>
+        <v>43692</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -33634,50 +33582,50 @@
         <v>9</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>15.99</v>
+        <v>4.99</v>
       </c>
       <c r="H17" s="8" t="n">
-        <v>255.84</v>
+        <v>174.65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4" t="n">
-        <v>43743</v>
+        <v>43709</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G18" s="7" t="n">
-        <v>8.99</v>
+        <v>125</v>
       </c>
       <c r="H18" s="8" t="n">
-        <v>251.72</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="n">
-        <v>43760</v>
+        <v>43726</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
@@ -33686,518 +33634,518 @@
         <v>9</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="G19" s="7" t="n">
-        <v>8.99</v>
+        <v>15.99</v>
       </c>
       <c r="H19" s="8" t="n">
-        <v>575.36</v>
+        <v>255.84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4" t="n">
-        <v>43777</v>
+        <v>43743</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>19.99</v>
+        <v>8.99</v>
       </c>
       <c r="H20" s="8" t="n">
-        <v>299.85</v>
+        <v>251.72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="n">
-        <v>43794</v>
+        <v>43760</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G21" s="7" t="n">
-        <v>4.99</v>
+        <v>8.99</v>
       </c>
       <c r="H21" s="8" t="n">
-        <v>479.04</v>
+        <v>575.36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="n">
-        <v>43811</v>
+        <v>43777</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>1.29</v>
+        <v>19.99</v>
       </c>
       <c r="H22" s="8" t="n">
-        <v>86.43</v>
+        <v>299.85</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="4" t="n">
-        <v>43828</v>
+        <v>43794</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>15.99</v>
+        <v>4.99</v>
       </c>
       <c r="H23" s="8" t="n">
-        <v>1183.26</v>
+        <v>479.04</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4" t="n">
-        <v>43845</v>
+        <v>43811</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="G24" s="7" t="n">
-        <v>8.99</v>
+        <v>1.29</v>
       </c>
       <c r="H24" s="8" t="n">
-        <v>413.54</v>
+        <v>86.43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4" t="n">
-        <v>43862</v>
+        <v>43828</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>15</v>
+        <v>15.99</v>
       </c>
       <c r="H25" s="8" t="n">
-        <v>1305</v>
+        <v>1183.26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4" t="n">
-        <v>43879</v>
+        <v>43845</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>4.99</v>
+        <v>8.99</v>
       </c>
       <c r="H26" s="8" t="n">
-        <v>19.96</v>
+        <v>413.54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="4" t="n">
-        <v>43897</v>
+        <v>43862</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="G27" s="7" t="n">
-        <v>19.99</v>
+        <v>15</v>
       </c>
       <c r="H27" s="8" t="n">
-        <v>139.93</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4" t="n">
-        <v>43914</v>
+        <v>43879</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="G28" s="7" t="n">
         <v>4.99</v>
       </c>
       <c r="H28" s="8" t="n">
-        <v>249.5</v>
+        <v>19.96</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4" t="n">
-        <v>43931</v>
+        <v>43897</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>1.99</v>
+        <v>19.99</v>
       </c>
       <c r="H29" s="8" t="n">
-        <v>131.34</v>
+        <v>139.93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="n">
-        <v>43948</v>
+        <v>43914</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="G30" s="7" t="n">
         <v>4.99</v>
       </c>
       <c r="H30" s="8" t="n">
-        <v>479.04</v>
+        <v>249.5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" s="4" t="n">
-        <v>43965</v>
+        <v>43931</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>1.29</v>
+        <v>1.99</v>
       </c>
       <c r="H31" s="8" t="n">
-        <v>68.37</v>
+        <v>131.34</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4" t="n">
-        <v>43982</v>
+        <v>43948</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>8.99</v>
+        <v>4.99</v>
       </c>
       <c r="H32" s="8" t="n">
-        <v>719.2</v>
+        <v>479.04</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4" t="n">
-        <v>43999</v>
+        <v>43965</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>125</v>
+        <v>1.29</v>
       </c>
       <c r="H33" s="8" t="n">
-        <v>625</v>
+        <v>68.37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4" t="n">
-        <v>44016</v>
+        <v>43982</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="G34" s="7" t="n">
-        <v>4.99</v>
+        <v>8.99</v>
       </c>
       <c r="H34" s="8" t="n">
-        <v>309.38</v>
+        <v>719.2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="4" t="n">
-        <v>44033</v>
+        <v>43999</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="G35" s="7" t="n">
-        <v>12.49</v>
+        <v>125</v>
       </c>
       <c r="H35" s="8" t="n">
-        <v>686.95</v>
+        <v>625</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4" t="n">
-        <v>44050</v>
+        <v>44016</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>23.95</v>
+        <v>4.99</v>
       </c>
       <c r="H36" s="8" t="n">
-        <v>1005.9</v>
+        <v>309.38</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4" t="n">
-        <v>44067</v>
+        <v>44033</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F37" s="5" t="n">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="G37" s="7" t="n">
-        <v>275</v>
+        <v>12.49</v>
       </c>
       <c r="H37" s="8" t="n">
-        <v>825</v>
+        <v>686.95</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4" t="n">
-        <v>44084</v>
+        <v>44050</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>1.29</v>
+        <v>23.95</v>
       </c>
       <c r="H38" s="8" t="n">
-        <v>9.03</v>
+        <v>1005.9</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="n">
-        <v>44101</v>
+        <v>44067</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>16</v>
@@ -34206,145 +34154,197 @@
         <v>17</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="G39" s="7" t="n">
-        <v>1.99</v>
+        <v>275</v>
       </c>
       <c r="H39" s="8" t="n">
-        <v>151.24</v>
+        <v>825</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4" t="n">
-        <v>44118</v>
+        <v>44084</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="G40" s="7" t="n">
-        <v>19.99</v>
+        <v>1.29</v>
       </c>
       <c r="H40" s="8" t="n">
-        <v>1139.43</v>
+        <v>9.03</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="4" t="n">
-        <v>44135</v>
+        <v>44101</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="G41" s="7" t="n">
-        <v>1.29</v>
+        <v>1.99</v>
       </c>
       <c r="H41" s="8" t="n">
-        <v>18.06</v>
+        <v>151.24</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="4" t="n">
-        <v>44152</v>
+        <v>44118</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>4.99</v>
+        <v>19.99</v>
       </c>
       <c r="H42" s="8" t="n">
-        <v>54.89</v>
+        <v>1139.43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="4" t="n">
-        <v>44169</v>
+        <v>44135</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="5" t="n">
-        <v>94</v>
-      </c>
       <c r="G43" s="7" t="n">
-        <v>19.99</v>
+        <v>1.29</v>
       </c>
       <c r="H43" s="8" t="n">
-        <v>1879.06</v>
+        <v>18.06</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="4" t="n">
-        <v>44186</v>
+        <v>44152</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="5" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G44" s="7" t="n">
         <v>4.99</v>
       </c>
       <c r="H44" s="8" t="n">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B45" s="4" t="n">
+        <v>44169</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>94</v>
+      </c>
+      <c r="G45" s="7" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="H45" s="8" t="n">
+        <v>1879.06</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B46" s="4" t="n">
+        <v>44186</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="G46" s="7" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H46" s="8" t="n">
         <v>139.72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merge changes from compat_py3.6-3.7 branch
</commit_message>
<xml_diff>
--- a/tests/samples/SampleData.xlsx
+++ b/tests/samples/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" state="visible" r:id="rId2"/>
@@ -406,9 +406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>303120</xdr:colOff>
+      <xdr:colOff>302760</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -418,7 +418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533160" y="1114200"/>
-          <a:ext cx="918000" cy="765360"/>
+          <a:ext cx="917640" cy="765000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,11 +526,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -579,7 +579,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>20</v>
+        <v>1200</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>1.99</v>
@@ -1702,7 +1702,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>
@@ -2034,7 +2034,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.57"/>
@@ -5130,7 +5130,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.87"/>
@@ -33194,11 +33194,11 @@
   </sheetPr>
   <dimension ref="A3:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.54"/>

</xml_diff>